<commit_message>
[Widget] - Row & Column
</commit_message>
<xml_diff>
--- a/Tutorial #/Widget.xlsx
+++ b/Tutorial #/Widget.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F0342B-2E8E-4ACE-9C15-24D5B6B4AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0C706F-4C94-4983-8B8E-9FBF4FCB1E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Container" sheetId="1" r:id="rId1"/>
+    <sheet name="Row &amp; Column" sheetId="2" r:id="rId2"/>
+    <sheet name="Column" sheetId="3" r:id="rId3"/>
+    <sheet name="Row" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Container Widget</t>
     <phoneticPr fontId="3"/>
@@ -94,6 +97,72 @@
   </si>
   <si>
     <t xml:space="preserve">Container එකට alignment එකක් දුන්නම එක effect වෙන්නේ child ට </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Row &amp; Column Widget</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Row &amp; Column වල design වෙන්නේ ක්‍රම දෙකකට </t>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">දාන order එක අනුව තමයි design එක හැදෙන්නේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget එකක් දැම්මම එකට යටින් තමයි ඊලග widget එක replace වෙන්නේ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Row</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">item replace වෙන්නේ පැත්තෙන් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">එක පේළියක විතරයි row එකක design එක වෙන්නේ </t>
+  </si>
+  <si>
+    <t>Column Widget</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>mainAxisAlignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">මෙහෙම center කලාට output center වෙලා එන්නේ නැ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපි එක check කරන්න background display කරමු </t>
+  </si>
+  <si>
+    <t xml:space="preserve">දැන් මෙතන පේනවා column එකේ පළල ඇවිත් තියෙන්නේ children widget එකේ පළලමයි </t>
+  </si>
+  <si>
+    <t>crossAxisAlignment</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒ නිසා crossAxisAlignment එකෙන් center කලාට එක display වෙන්න ඉඩක් එකක් නැ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">width එක වැඩි කලොත් text එක center වෙනවා </t>
+  </si>
+  <si>
+    <t>Row Widget</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Column code එකම row කියලා rename කරගනිමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Item replace වෙන්නේ පැත්තෙන් </t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -101,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +208,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF00B050"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color rgb="FF002060"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF00B050"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF002060"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,13 +265,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,6 +1214,901 @@
         <a:xfrm>
           <a:off x="6911340" y="41781438"/>
           <a:ext cx="3632279" cy="3025603"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>206896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>300292</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5FE3713-A417-13E3-A438-41982191A7E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="883920" y="1677556"/>
+          <a:ext cx="6057900" cy="3796716"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>42179</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>252826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F50821A3-CBBA-41D0-AD0F-BB69DB4B479B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="701040" y="2987040"/>
+          <a:ext cx="4035059" cy="3468466"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>45129</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62300CC1-CBB3-49AB-93ED-E8023BE6730F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5379720" y="3368040"/>
+          <a:ext cx="4723809" cy="2580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>53341</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>340464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>251461</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>386254</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{050B36AE-27D7-81A5-0C2A-5B3934906A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723901" y="7236564"/>
+          <a:ext cx="4892040" cy="2926150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>669697</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>410418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2847D8-9F0F-5B82-F130-8130CBA6DB97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6034177" y="6256020"/>
+          <a:ext cx="2013904" cy="3930858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>200522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>89136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A447D546-52AE-7936-8B23-CD6FC5929946}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="746760" y="11211422"/>
+          <a:ext cx="4785360" cy="2357494"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>432909</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>335280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>204878</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{444B2E31-0716-F795-0F27-DA045DF73292}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5797389" y="10523220"/>
+          <a:ext cx="2260216" cy="3572918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>391637</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>356012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47CBA974-AC94-FBE1-A314-B0E87E8EF8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="754380" y="15544800"/>
+          <a:ext cx="6342857" cy="1780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254216</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>35175</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>326798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{987C0F80-3A27-41C0-8BA6-96C7B8055DB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7630376" y="14874240"/>
+          <a:ext cx="1792639" cy="2833778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>24216</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>251189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EBB44FC-8797-1BF9-D953-FCD669009E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="998220" y="19575780"/>
+          <a:ext cx="4390476" cy="2171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>138787</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>317597</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>317293</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C657953-1D4B-1180-8D18-7C0CEA7DAE1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6173827" y="18790920"/>
+          <a:ext cx="2190490" cy="3433873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>335280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50622</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>85448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B5CB0C2-0C12-7BA1-B59E-9C5C8B6DB7E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="922020" y="23888700"/>
+          <a:ext cx="6504762" cy="2219048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>652728</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>670559</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>39860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83F44D83-352E-A9F4-8717-6E1EA488204D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8028888" y="23301960"/>
+          <a:ext cx="2029511" cy="3171680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>632461</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>601035</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0240B0EC-C1DB-4EDA-E967-707DF0E5052A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="632461" y="2743200"/>
+          <a:ext cx="3991934" cy="5326380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>453698</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>372073</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F37C7018-465A-2FBB-48B9-CF2336E8D23A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5147618" y="2750820"/>
+          <a:ext cx="3941735" cy="5318760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289012</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>20651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDDBF14B-F711-655E-BB4B-8416608910E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2613660" y="8580120"/>
+          <a:ext cx="4380952" cy="2428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>51357</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>52354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FF96B06-1DC9-8029-9678-735735628B5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="815340" y="11628120"/>
+          <a:ext cx="4600497" cy="4761514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>24916</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>312420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>348980</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>403860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D28355A-0349-E6D5-BB2F-A46FF7E2EEAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6059956" y="12123420"/>
+          <a:ext cx="3676864" cy="3794760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>220113</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>304619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30ED128C-B689-00F9-53A7-E91762B4B8B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="662940" y="17663160"/>
+          <a:ext cx="6933333" cy="1447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>387194</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>53339</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>300889</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C53F42C4-856F-834B-042B-E646D96FE63A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7763354" y="16390619"/>
+          <a:ext cx="2592226" cy="3950870"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1378,7 +2385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>
@@ -1490,4 +2497,179 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52127678-77FA-4EB4-972D-B012AB27CFD8}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.8">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="58.2" x14ac:dyDescent="1.4">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B17" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.8"/>
+    <row r="19" spans="1:2" ht="58.2" x14ac:dyDescent="1.4">
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A23" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6DD4C3-6B9C-453E-836F-BB2137722312}">
+  <dimension ref="A1:B56"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.8">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.8"/>
+    <row r="16" spans="1:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B16" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B36" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B44" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B54" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B55" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B56" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912DDF8A-7585-403B-8525-25080E43D7C1}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.8">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.8">
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B6" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Flutter] - Create a new screen
</commit_message>
<xml_diff>
--- a/Tutorial #/Widget.xlsx
+++ b/Tutorial #/Widget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA6C3DB-C8B9-4615-98C4-DB1297FD33A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAFA0A5-0546-4D22-AF72-6EA3488C1C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Container Widget</t>
     <phoneticPr fontId="3"/>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve">මේ ගැටලුව විසදන්න Stateful use කරන්න පුළුවන් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේ දෙක දාන්න කලින් හරියටම දාන්න ඕන මොකක්ද කියලා තීරණය කරන්න </t>
   </si>
 </sst>
 </file>
@@ -2605,7 +2608,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -2643,7 +2646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2949,10 +2952,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -3035,9 +3038,15 @@
         <v>47</v>
       </c>
     </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="B22" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[TextField] - Get user input data
</commit_message>
<xml_diff>
--- a/Tutorial #/Widget.xlsx
+++ b/Tutorial #/Widget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A96D80B-A914-4E1B-B3FD-9D4E5CB6F797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439C2166-B20B-4519-B5B2-F65CE052ECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Container Widget</t>
     <phoneticPr fontId="3"/>
@@ -260,13 +260,28 @@
   <si>
     <t xml:space="preserve">Value ගොඩක් ගන්නවානම් Text form field use කරනවා </t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User input data අරගන්නේ කොහොමද කියලා බලමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>onChanged</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>onSubmitted</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">type කරලා submit කලාට පස්සේ තමයි print වෙන්නේ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,13 +391,27 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF002060"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -397,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -427,6 +456,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2492,6 +2524,270 @@
         <a:xfrm>
           <a:off x="6187440" y="5912829"/>
           <a:ext cx="3868494" cy="1839793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>68579</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>358358</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4EEF855-139C-9A2E-547C-F10BB1A76781}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="563879" y="10073640"/>
+          <a:ext cx="4983699" cy="4213860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>487244</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>525780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>165145</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>64353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{470258D7-BD7D-AD11-47DB-BD856E80DA05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6347024" y="9814560"/>
+          <a:ext cx="3701261" cy="2617053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>358140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>429951</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EBF36F-1883-295C-6358-E1CF84C6D94C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7696200" y="11902440"/>
+          <a:ext cx="4628571" cy="2238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>144781</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>272291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>175261</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>273929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3264349A-F788-2F27-E26E-30C9354C4A5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640081" y="16129511"/>
+          <a:ext cx="5394960" cy="2881998"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>195872</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CBDCCF-86DE-9B7E-2A38-BA172481E5E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6576060" y="16002000"/>
+          <a:ext cx="2895600" cy="1697012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>396240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>650969</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>207463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078A0EB4-AAE1-5750-D116-EA06BE03E26E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7551420" y="17487900"/>
+          <a:ext cx="4323809" cy="1457143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3218,10 +3514,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -3266,7 +3562,45 @@
         <v>63</v>
       </c>
     </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.8">
+      <c r="B21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B23" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="36" spans="2:9" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B36" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.8">
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B36:I36"/>
+  </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>